<commit_message>
edits to Prefetch and Hold ops
</commit_message>
<xml_diff>
--- a/docs/argo-sub-notif.xlsx
+++ b/docs/argo-sub-notif.xlsx
@@ -459,7 +459,7 @@
     <t>trigger-description</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {[CanonicalType[http://fhir.org/guides/argonaut-scheduling/StructureDefinition/extension-trigger-event]]} {[]}
+    <t xml:space="preserve">Extension {[CanonicalType[http://fhir.org/guides/argonaut-scheduling/StructureDefinition/extension-subscription-triggerevent]]} {[]}
 </t>
   </si>
   <si>
@@ -487,13 +487,13 @@
     <t>Subscription Trigger Event FHIRPath Extension</t>
   </si>
   <si>
-    <t>If the expression is a [FHIRPath](http://hl7.org/fhirpath/) expression, it evaluates in the context of a resource of one of the types identified in the [Subscription Event Focus Extension](StructureDefinition-extension-event-focus.html), and may also refer to the variable `%previous`  for delta comparisons.</t>
+    <t>If the expression is a [FHIRPath](http://hl7.org/fhirpath/) expression, it evaluates in the context of a resource of one of the types identified in the [Subscription Event Focus Extension](StructureDefinition-extension-subscription-eventfocus.html), and may also refer to the variable `%previous`  for delta comparisons.</t>
   </si>
   <si>
     <t>event-focus</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {[CanonicalType[http://fhir.org/guides/argonaut-scheduling/StructureDefinition/extension-event-focus]]} {[]}
+    <t xml:space="preserve">Extension {[CanonicalType[http://fhir.org/guides/argonaut-scheduling/StructureDefinition/extension-subscription-eventfocus]]} {[]}
 </t>
   </si>
   <si>
@@ -533,7 +533,7 @@
     <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
   </si>
   <si>
-    <t>&lt;valueUri xmlns="http://hl7.org/fhir" value="http://fhir.org/guides/argonaut-scheduling/StructureDefinition/extension-event-focus"/&gt;</t>
+    <t>&lt;valueUri xmlns="http://hl7.org/fhir" value="http://fhir.org/guides/argonaut-scheduling/StructureDefinition/extension-subscription-eventfocus"/&gt;</t>
   </si>
   <si>
     <t>Extension.url</t>
@@ -617,7 +617,7 @@
     <t>payload-profile</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {[CanonicalType[http://fhir.org/guides/argonaut-scheduling/StructureDefinition/extension-payload-profile]]} {[]}
+    <t xml:space="preserve">Extension {[CanonicalType[http://fhir.org/guides/argonaut-scheduling/StructureDefinition/extension-subscription-payloadprofile]]} {[]}
 </t>
   </si>
   <si>
@@ -634,7 +634,7 @@
     <t>Subscription.channel.extension.url</t>
   </si>
   <si>
-    <t>&lt;valueUri xmlns="http://hl7.org/fhir" value="http://fhir.org/guides/argonaut-scheduling/StructureDefinition/extension-payload-profile"/&gt;</t>
+    <t>&lt;valueUri xmlns="http://hl7.org/fhir" value="http://fhir.org/guides/argonaut-scheduling/StructureDefinition/extension-subscription-payloadprofile"/&gt;</t>
   </si>
   <si>
     <t>Subscription.channel.extension.valueUri</t>

</xml_diff>